<commit_message>
:sparkle: Problem 101 solved
</commit_message>
<xml_diff>
--- a/Question List/FINAL450.xlsx
+++ b/Question List/FINAL450.xlsx
@@ -1665,11 +1665,11 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B67" activeCellId="0" sqref="B67"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C57" activeCellId="0" sqref="C57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -2245,7 +2245,7 @@
         <v>57</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2712,7 +2712,7 @@
         <v>100</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>